<commit_message>
This is just to save the work I'm currently doing. I'm trying to fix the spacing between the grid squares before we go and duplicate this for Electrical, Mechanical, etc. I'm also trying to ensure the code that shifts the columns from 2 to 1 (when screen size is not big) works. Suggestions are always welcome! :)
</commit_message>
<xml_diff>
--- a/docs/Projects-Information.xlsx
+++ b/docs/Projects-Information.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markd\OneDrive - University of Guelph\Robotics Stuff\ugrt.github.io\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C81EEF6-CB5B-47D7-A416-2756DAEBB15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D2FBCA91-74CD-4D43-8546-5A48645A73C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D53B2B5F-B801-4133-BE6F-33CB08000367}"/>
   <bookViews>
-    <workbookView xWindow="11110" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Electrical" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -53,9 +54,6 @@
     <t>Electrical</t>
   </si>
   <si>
-    <t>electrical</t>
-  </si>
-  <si>
     <t>The electrical team is responsible for creating the electrical system of the rover and interfacing it with the mechanical and programming teams</t>
   </si>
   <si>
@@ -65,9 +63,6 @@
     <t>Mechanical</t>
   </si>
   <si>
-    <t>mechanical</t>
-  </si>
-  <si>
     <t>The mechanical team is responsible for creating the chassis of the rover as well as coordinating all the moving components.</t>
   </si>
   <si>
@@ -80,9 +75,6 @@
     <t>Programming</t>
   </si>
   <si>
-    <t>programming</t>
-  </si>
-  <si>
     <t>craxy, no?</t>
   </si>
   <si>
@@ -98,18 +90,49 @@
     <t>Marketing</t>
   </si>
   <si>
-    <t>marketing</t>
-  </si>
-  <si>
-    <t>The marketing team is required to create all the information we have available on the website. They go out and find sponsors as well as coordonate and manage our social medias.</t>
+    <r>
+      <t xml:space="preserve">The marketing team is required to create all the information we have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>available</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on the website. They go out and find sponsors as well as coordonate and manage our social medias.</t>
+    </r>
+  </si>
+  <si>
+    <t>Project Title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -479,7 +502,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,75 +526,180 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1" t="str">
+        <f>LOWER(A2)</f>
+        <v>electrical</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f t="shared" ref="B3:B5" si="0">LOWER(A3)</f>
+        <v>mechanical</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>programming</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>marketing</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75AA5DD-3E6F-47C8-950F-B05F77975122}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="26" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>LOWER(A2)</f>
+        <v>electrical</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="str">
+        <f t="shared" ref="B3:B5" si="0">LOWER(A3)</f>
+        <v/>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On paper, I deleted the letter c from the projects grid. Really, I tried playing with colours and how everything works. I added the colours as variables and put the solid and transparent versions of all 4. The colours are brutal and it might take a meeting with a few of us to figure out good colour layering and what we want it to look like.
</commit_message>
<xml_diff>
--- a/docs/Projects-Information.xlsx
+++ b/docs/Projects-Information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D2FBCA91-74CD-4D43-8546-5A48645A73C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D53B2B5F-B801-4133-BE6F-33CB08000367}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{D2FBCA91-74CD-4D43-8546-5A48645A73C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4235836A-7774-497A-A7D3-0CB1994829E5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="5600" yWindow="2170" windowWidth="16800" windowHeight="9670" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>Title</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Project Title</t>
+  </si>
+  <si>
+    <t>/images/it in the hall.jpg</t>
   </si>
 </sst>
 </file>
@@ -501,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2CFC88-1D52-4579-843F-FBBB9CB93435}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,7 +547,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
I introduced dynamic URLs into the website so that we can create new projects and have the URLs match the title. Still in testing.
</commit_message>
<xml_diff>
--- a/docs/Projects-Information.xlsx
+++ b/docs/Projects-Information.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{D2FBCA91-74CD-4D43-8546-5A48645A73C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4235836A-7774-497A-A7D3-0CB1994829E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="2170" windowWidth="16800" windowHeight="9670" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Projects" sheetId="1" r:id="rId1"/>
     <sheet name="Electrical" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -126,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,18 +505,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2CFC88-1D52-4579-843F-FBBB9CB93435}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" style="1" customWidth="1"/>
     <col min="3" max="16384" width="26" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="84">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,12 +551,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="70">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f t="shared" ref="B3:B5" si="0">LOWER(A3)</f>
+        <f>LOWER(A3)</f>
         <v>mechanical</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -568,12 +569,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="28">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>LOWER(A4)</f>
         <v>programming</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -586,12 +587,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="84">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>LOWER(A5)</f>
         <v>marketing</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -618,14 +619,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" style="1" customWidth="1"/>
     <col min="3" max="16384" width="26" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -642,7 +643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="84">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -660,9 +661,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="70">
       <c r="B3" s="1" t="str">
-        <f t="shared" ref="B3:B5" si="0">LOWER(A3)</f>
+        <f>LOWER(A3)</f>
         <v/>
       </c>
       <c r="C3" s="1" t="s">
@@ -675,9 +676,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="28">
       <c r="B4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>LOWER(A4)</f>
         <v/>
       </c>
       <c r="C4" s="1" t="s">
@@ -690,9 +691,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="84">
       <c r="B5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>LOWER(A5)</f>
         <v/>
       </c>
       <c r="C5" s="1" t="s">
@@ -709,4 +710,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{be62a12b-2cad-49a1-a5fa-85f4f3156a7d}" enabled="0" method="" siteId="{be62a12b-2cad-49a1-a5fa-85f4f3156a7d}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
This is with the addition of the subteam page. Still in the development stages, but is working well.
</commit_message>
<xml_diff>
--- a/docs/Projects-Information.xlsx
+++ b/docs/Projects-Information.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADA5658A-9505-4B88-AC84-CA0B9DF6A3F6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="1" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
     <sheet name="Electrical" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Title</t>
   </si>
@@ -122,12 +121,48 @@
   <si>
     <t>/images/it in the hall.jpg</t>
   </si>
+  <si>
+    <t>Project 1</t>
+  </si>
+  <si>
+    <t>Project 2</t>
+  </si>
+  <si>
+    <t>Project 3</t>
+  </si>
+  <si>
+    <t>Project 4</t>
+  </si>
+  <si>
+    <t>This is project 1</t>
+  </si>
+  <si>
+    <t>This is project 2</t>
+  </si>
+  <si>
+    <t>This is project 3</t>
+  </si>
+  <si>
+    <t>This is project 4</t>
+  </si>
+  <si>
+    <t>big blurb for project 1</t>
+  </si>
+  <si>
+    <t>big blurb for project 2</t>
+  </si>
+  <si>
+    <t>big blurb for project 3</t>
+  </si>
+  <si>
+    <t>big blurb for project 4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +174,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,18 +546,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2CFC88-1D52-4579-843F-FBBB9CB93435}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="26" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="84">
+    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -551,7 +592,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="70">
+    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -569,7 +610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -587,7 +628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="84">
+    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -615,18 +656,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75AA5DD-3E6F-47C8-950F-B05F77975122}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="26" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -643,70 +684,80 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="84">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>LOWER(A2)</f>
-        <v>electrical</v>
+        <v>project 1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="70">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B3" s="1" t="str">
         <f>LOWER(A3)</f>
-        <v/>
+        <v>project 2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" s="1" t="str">
         <f>LOWER(A4)</f>
-        <v/>
+        <v>project 3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="84">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B5" s="1" t="str">
         <f>LOWER(A5)</f>
-        <v/>
+        <v>project 4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the files to be more concise and have better names that reflected what they were actually for. I also update the URLs across the site to use the word subteams instead of projects. This is bc we are now having subteam pgs and containing the individual projects in each subteam pg.
</commit_message>
<xml_diff>
--- a/docs/Projects-Information.xlsx
+++ b/docs/Projects-Information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADA5658A-9505-4B88-AC84-CA0B9DF6A3F6}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8BAD6DD-6046-4182-BA03-33447DD8A71E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="1" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="11110" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>little title</t>
   </si>
@@ -90,32 +87,6 @@
     <t>Marketing</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The marketing team is required to create all the information we have </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>available</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> on the website. They go out and find sponsors as well as coordonate and manage our social medias.</t>
-    </r>
-  </si>
-  <si>
     <t>Project Title</t>
   </si>
   <si>
@@ -156,22 +127,53 @@
   </si>
   <si>
     <t>big blurb for project 4</t>
+  </si>
+  <si>
+    <t>Project 5</t>
+  </si>
+  <si>
+    <t>This is project 5</t>
+  </si>
+  <si>
+    <t>big blurb for project 5</t>
+  </si>
+  <si>
+    <t>Project 6</t>
+  </si>
+  <si>
+    <t>This is project 6</t>
+  </si>
+  <si>
+    <t>big blurb for project 6</t>
+  </si>
+  <si>
+    <t>imgPath</t>
+  </si>
+  <si>
+    <t>subpageFn</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>littleTitle</t>
+  </si>
+  <si>
+    <t>littleBlurb</t>
+  </si>
+  <si>
+    <t>bigBlurb</t>
+  </si>
+  <si>
+    <t>The marketing team is required to create all the information we have available on the website. They go out and find sponsors as well as coordonate and manage our social medias.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -205,9 +207,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -544,10 +549,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2CFC88-1D52-4579-843F-FBBB9CB93435}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="26" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>LOWER(A2)</f>
+        <v>electrical</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>_xlfn.CONCAT(B2,"Projects")</f>
+        <v>electricalProjects</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>LOWER(A3)</f>
+        <v>mechanical</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F5" si="0">_xlfn.CONCAT(B3,"Projects")</f>
+        <v>mechanicalProjects</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>LOWER(A4)</f>
+        <v>programming</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>programmingProjects</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>LOWER(A5)</f>
+        <v>marketing</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>marketingProjects</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75AA5DD-3E6F-47C8-950F-B05F77975122}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -559,205 +693,131 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <f>LOWER(A2)</f>
-        <v>electrical</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="str">
-        <f>LOWER(A3)</f>
-        <v>mechanical</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f>LOWER(A4)</f>
-        <v>programming</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <f>LOWER(A5)</f>
-        <v>marketing</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75AA5DD-3E6F-47C8-950F-B05F77975122}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="26" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f>LOWER(A2)</f>
+        <f t="shared" ref="B2:B7" si="0">LOWER(A2)</f>
         <v>project 1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>LOWER(A3)</f>
+        <f t="shared" si="0"/>
         <v>project 2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f>LOWER(A4)</f>
+        <f t="shared" si="0"/>
         <v>project 3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="str">
-        <f>LOWER(A5)</f>
+        <f t="shared" si="0"/>
         <v>project 4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>project 5</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>project 6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed the way we make headers. This should make it easier to create headers bc we have the help of the IDE. The JS doc will also allow us to createe footers when the time comes. This has only been implemented on the About Us page so it will need to be distributed across the rest of the pages.
</commit_message>
<xml_diff>
--- a/docs/Projects-Information.xlsx
+++ b/docs/Projects-Information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8BAD6DD-6046-4182-BA03-33447DD8A71E}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9EFF742-934E-4690-9BA9-4AF65C94C126}"/>
   <bookViews>
-    <workbookView xWindow="11110" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="-3560" yWindow="-10890" windowWidth="19380" windowHeight="10260" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -37,16 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
-  <si>
-    <t>little title</t>
-  </si>
-  <si>
-    <t>Little Blurb</t>
-  </si>
-  <si>
-    <t>BIG BLURB</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Electrical</t>
   </si>
@@ -78,18 +69,12 @@
     <t>Lets see if me updating this changes the shit…</t>
   </si>
   <si>
-    <t>Image path</t>
-  </si>
-  <si>
     <t xml:space="preserve">url_for('static',filename='it in the hall.jpg') </t>
   </si>
   <si>
     <t>Marketing</t>
   </si>
   <si>
-    <t>Project Title</t>
-  </si>
-  <si>
     <t>/images/it in the hall.jpg</t>
   </si>
   <si>
@@ -166,12 +151,21 @@
   </si>
   <si>
     <t>The marketing team is required to create all the information we have available on the website. They go out and find sponsors as well as coordonate and manage our social medias.</t>
+  </si>
+  <si>
+    <t>thinkg</t>
+  </si>
+  <si>
+    <t>bigBlurb2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;/images&quot;\+"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -212,9 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -230,6 +222,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -549,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2CFC88-1D52-4579-843F-FBBB9CB93435}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,110 +558,113 @@
     <col min="3" max="16384" width="26" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>LOWER(A2)</f>
         <v>electrical</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="str">
         <f>_xlfn.CONCAT(B2,"Projects")</f>
         <v>electricalProjects</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="str">
         <f>LOWER(A3)</f>
         <v>mechanical</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f t="shared" ref="G3:G5" si="0">_xlfn.CONCAT(B3,"Projects")</f>
+        <v>mechanicalProjects</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="str">
-        <f t="shared" ref="F3:F5" si="0">_xlfn.CONCAT(B3,"Projects")</f>
-        <v>mechanicalProjects</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>LOWER(A4)</f>
         <v>programming</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="str">
+      <c r="G4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>programmingProjects</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>LOWER(A5)</f>
         <v>marketing</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>42</v>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="str">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>marketingProjects</v>
       </c>
@@ -678,10 +677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75AA5DD-3E6F-47C8-950F-B05F77975122}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,129 +690,166 @@
     <col min="3" max="16384" width="26" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>Projects!A$1</f>
+        <v>title</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>Projects!B$1</f>
+        <v>littleTitle</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f>Projects!C$1</f>
+        <v>littleBlurb</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f>Projects!D$1</f>
+        <v>bigBlurb</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f>Projects!E$1</f>
+        <v>bigBlurb2</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f>Projects!F$1</f>
+        <v>imgPath</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f>Projects!G$1</f>
+        <v>subpageFn</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="B2" s="1" t="str">
         <f t="shared" ref="B2:B7" si="0">LOWER(A2)</f>
         <v>project 1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>_xlfn.CONCAT(LOWER($E$1), " for ",B2)</f>
+        <v>bigblurb2 for project 1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f t="shared" ref="E3:E7" si="1">_xlfn.CONCAT(LOWER($E$1), " for ",B3)</f>
+        <v>bigblurb2 for project 2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>bigblurb2 for project 3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 4</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>bigblurb2 for project 4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>bigblurb2 for project 5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>bigblurb2 for project 6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I went and cleaned up all the documents and removed the unused spacing and code.
</commit_message>
<xml_diff>
--- a/docs/Projects-Information.xlsx
+++ b/docs/Projects-Information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/delimam_uoguelph_ca/Documents/Robotics Stuff/ugrt.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9EFF742-934E-4690-9BA9-4AF65C94C126}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{479BD6A4-6BBC-427A-9470-0DE38B9D4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52030137-C79D-4B27-B40E-37327F31ACAB}"/>
   <bookViews>
-    <workbookView xWindow="-3560" yWindow="-10890" windowWidth="19380" windowHeight="10260" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="1" xr2:uid="{850585D9-EA53-420A-A917-69AE9798DAAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -78,12 +78,6 @@
     <t>/images/it in the hall.jpg</t>
   </si>
   <si>
-    <t>Project 1</t>
-  </si>
-  <si>
-    <t>Project 2</t>
-  </si>
-  <si>
     <t>Project 3</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>bigBlurb2</t>
+  </si>
+  <si>
+    <t>Project1</t>
+  </si>
+  <si>
+    <t>Project2</t>
   </si>
 </sst>
 </file>
@@ -222,10 +222,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -547,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2CFC88-1D52-4579-843F-FBBB9CB93435}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -560,25 +556,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="87" x14ac:dyDescent="0.35">
@@ -596,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1" t="str">
         <f>_xlfn.CONCAT(B2,"Projects")</f>
@@ -656,7 +652,7 @@
         <v>marketing</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -679,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75AA5DD-3E6F-47C8-950F-B05F77975122}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -722,21 +718,21 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f t="shared" ref="B2:B7" si="0">LOWER(A2)</f>
-        <v>project 1</v>
+        <f>LOWER(A2)</f>
+        <v>project1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="str">
         <f>_xlfn.CONCAT(LOWER($E$1), " for ",B2)</f>
-        <v>bigblurb2 for project 1</v>
+        <v>bigblurb2 for project1</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -744,21 +740,21 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>project 2</v>
+        <f t="shared" ref="B2:B7" si="0">LOWER(A3)</f>
+        <v>project2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="str">
         <f t="shared" ref="E3:E7" si="1">_xlfn.CONCAT(LOWER($E$1), " for ",B3)</f>
-        <v>bigblurb2 for project 2</v>
+        <v>bigblurb2 for project2</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -766,17 +762,17 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="1"/>
@@ -788,17 +784,17 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -810,17 +806,17 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="1"/>
@@ -832,17 +828,17 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>project 6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="1"/>

</xml_diff>